<commit_message>
Add doc of Sunrise / Sunset difference among Yahoo / Open / Wunder.
</commit_message>
<xml_diff>
--- a/doc/wunderground_お天気一覧.xlsx
+++ b/doc/wunderground_お天気一覧.xlsx
@@ -1249,16 +1249,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6515,56 +6515,6 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="6762750" y="13230225"/>
-          <a:ext cx="476250" cy="476250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="476250" cy="476250"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="100" name="図 99" descr="http://icons.wxug.com/i/c/c/cloudy.gif"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6762750" y="13735050"/>
           <a:ext cx="476250" cy="476250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8905,9 +8855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8921,23 +8869,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="F2" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="K2" s="8" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="K2" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
     </row>
     <row r="3" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
@@ -8958,7 +8906,7 @@
       <c r="H3" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="8" t="s">
         <v>268</v>
       </c>
       <c r="K3" s="3" t="s">
@@ -8970,7 +8918,7 @@
       <c r="M3" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="8" t="s">
         <v>268</v>
       </c>
     </row>
@@ -8989,7 +8937,7 @@
         <v>237</v>
       </c>
       <c r="H4" s="6"/>
-      <c r="I4" s="9">
+      <c r="I4" s="7">
         <v>22</v>
       </c>
       <c r="K4" s="6" t="s">
@@ -8999,7 +8947,7 @@
         <v>273</v>
       </c>
       <c r="M4" s="6"/>
-      <c r="N4" s="9">
+      <c r="N4" s="7">
         <v>1</v>
       </c>
     </row>
@@ -9018,7 +8966,7 @@
         <v>238</v>
       </c>
       <c r="H5" s="6"/>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
         <v>12</v>
       </c>
       <c r="K5" s="6" t="s">
@@ -9028,7 +8976,7 @@
         <v>262</v>
       </c>
       <c r="M5" s="6"/>
-      <c r="N5" s="9">
+      <c r="N5" s="7">
         <v>1</v>
       </c>
     </row>
@@ -9047,7 +8995,7 @@
         <v>238</v>
       </c>
       <c r="H6" s="6"/>
-      <c r="I6" s="9">
+      <c r="I6" s="7">
         <v>12</v>
       </c>
       <c r="K6" s="6" t="s">
@@ -9057,7 +9005,7 @@
         <v>274</v>
       </c>
       <c r="M6" s="6"/>
-      <c r="N6" s="9">
+      <c r="N6" s="7">
         <v>2</v>
       </c>
     </row>
@@ -9076,7 +9024,7 @@
         <v>241</v>
       </c>
       <c r="H7" s="6"/>
-      <c r="I7" s="9">
+      <c r="I7" s="7">
         <v>22</v>
       </c>
       <c r="K7" s="6" t="s">
@@ -9086,7 +9034,7 @@
         <v>275</v>
       </c>
       <c r="M7" s="6"/>
-      <c r="N7" s="9">
+      <c r="N7" s="7">
         <v>2</v>
       </c>
     </row>
@@ -9105,7 +9053,7 @@
         <v>241</v>
       </c>
       <c r="H8" s="6"/>
-      <c r="I8" s="9">
+      <c r="I8" s="7">
         <v>22</v>
       </c>
       <c r="K8" s="6" t="s">
@@ -9115,7 +9063,7 @@
         <v>276</v>
       </c>
       <c r="M8" s="6"/>
-      <c r="N8" s="9">
+      <c r="N8" s="7">
         <v>3</v>
       </c>
     </row>
@@ -9134,7 +9082,7 @@
         <v>243</v>
       </c>
       <c r="H9" s="6"/>
-      <c r="I9" s="9">
+      <c r="I9" s="7">
         <v>20</v>
       </c>
       <c r="K9" s="6" t="s">
@@ -9144,7 +9092,7 @@
         <v>277</v>
       </c>
       <c r="M9" s="6"/>
-      <c r="N9" s="9">
+      <c r="N9" s="7">
         <v>3</v>
       </c>
     </row>
@@ -9163,7 +9111,7 @@
         <v>245</v>
       </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="9">
+      <c r="I10" s="7">
         <v>14</v>
       </c>
       <c r="K10" s="6" t="s">
@@ -9173,7 +9121,7 @@
         <v>278</v>
       </c>
       <c r="M10" s="6"/>
-      <c r="N10" s="9">
+      <c r="N10" s="7">
         <v>4</v>
       </c>
     </row>
@@ -9192,7 +9140,7 @@
         <v>245</v>
       </c>
       <c r="H11" s="6"/>
-      <c r="I11" s="9">
+      <c r="I11" s="7">
         <v>14</v>
       </c>
       <c r="K11" s="6" t="s">
@@ -9202,7 +9150,7 @@
         <v>279</v>
       </c>
       <c r="M11" s="6"/>
-      <c r="N11" s="9">
+      <c r="N11" s="7">
         <v>5</v>
       </c>
     </row>
@@ -9221,7 +9169,7 @@
         <v>246</v>
       </c>
       <c r="H12" s="6"/>
-      <c r="I12" s="9">
+      <c r="I12" s="7">
         <v>1</v>
       </c>
       <c r="K12" s="6" t="s">
@@ -9231,7 +9179,7 @@
         <v>280</v>
       </c>
       <c r="M12" s="6"/>
-      <c r="N12" s="9">
+      <c r="N12" s="7">
         <v>6</v>
       </c>
     </row>
@@ -9250,7 +9198,7 @@
         <v>247</v>
       </c>
       <c r="H13" s="6"/>
-      <c r="I13" s="9">
+      <c r="I13" s="7">
         <v>4</v>
       </c>
       <c r="K13" s="6" t="s">
@@ -9260,7 +9208,7 @@
         <v>271</v>
       </c>
       <c r="M13" s="6"/>
-      <c r="N13" s="9">
+      <c r="N13" s="7">
         <v>12</v>
       </c>
     </row>
@@ -9279,7 +9227,7 @@
         <v>248</v>
       </c>
       <c r="H14" s="6"/>
-      <c r="I14" s="9">
+      <c r="I14" s="7">
         <v>16</v>
       </c>
       <c r="K14" s="6" t="s">
@@ -9289,7 +9237,7 @@
         <v>281</v>
       </c>
       <c r="M14" s="6"/>
-      <c r="N14" s="9">
+      <c r="N14" s="7">
         <v>13</v>
       </c>
     </row>
@@ -9308,7 +9256,7 @@
         <v>249</v>
       </c>
       <c r="H15" s="6"/>
-      <c r="I15" s="9">
+      <c r="I15" s="7">
         <v>6</v>
       </c>
       <c r="K15" s="6" t="s">
@@ -9318,7 +9266,7 @@
         <v>282</v>
       </c>
       <c r="M15" s="6"/>
-      <c r="N15" s="9">
+      <c r="N15" s="7">
         <v>14</v>
       </c>
     </row>
@@ -9337,7 +9285,7 @@
         <v>250</v>
       </c>
       <c r="H16" s="6"/>
-      <c r="I16" s="9">
+      <c r="I16" s="7">
         <v>5</v>
       </c>
       <c r="K16" s="6" t="s">
@@ -9347,7 +9295,7 @@
         <v>283</v>
       </c>
       <c r="M16" s="6"/>
-      <c r="N16" s="9">
+      <c r="N16" s="7">
         <v>15</v>
       </c>
     </row>
@@ -9366,7 +9314,7 @@
         <v>251</v>
       </c>
       <c r="H17" s="6"/>
-      <c r="I17" s="9">
+      <c r="I17" s="7">
         <v>3</v>
       </c>
       <c r="K17" s="6" t="s">
@@ -9376,7 +9324,7 @@
         <v>284</v>
       </c>
       <c r="M17" s="6"/>
-      <c r="N17" s="9">
+      <c r="N17" s="7">
         <v>15</v>
       </c>
     </row>
@@ -9395,7 +9343,7 @@
         <v>253</v>
       </c>
       <c r="H18" s="6"/>
-      <c r="I18" s="9">
+      <c r="I18" s="7">
         <v>2</v>
       </c>
       <c r="K18" s="6" t="s">
@@ -9405,7 +9353,7 @@
         <v>285</v>
       </c>
       <c r="M18" s="6"/>
-      <c r="N18" s="9">
+      <c r="N18" s="7">
         <v>16</v>
       </c>
     </row>
@@ -9424,7 +9372,7 @@
         <v>254</v>
       </c>
       <c r="H19" s="6"/>
-      <c r="I19" s="9">
+      <c r="I19" s="7">
         <v>2</v>
       </c>
       <c r="K19" s="6" t="s">
@@ -9434,7 +9382,7 @@
         <v>286</v>
       </c>
       <c r="M19" s="6"/>
-      <c r="N19" s="9">
+      <c r="N19" s="7">
         <v>16</v>
       </c>
     </row>
@@ -9453,7 +9401,7 @@
         <v>256</v>
       </c>
       <c r="H20" s="6"/>
-      <c r="I20" s="9">
+      <c r="I20" s="7">
         <v>3</v>
       </c>
       <c r="K20" s="6" t="s">
@@ -9463,7 +9411,7 @@
         <v>287</v>
       </c>
       <c r="M20" s="6"/>
-      <c r="N20" s="9">
+      <c r="N20" s="7">
         <v>20</v>
       </c>
     </row>
@@ -9482,7 +9430,7 @@
         <v>257</v>
       </c>
       <c r="H21" s="6"/>
-      <c r="I21" s="9">
+      <c r="I21" s="7">
         <v>16</v>
       </c>
       <c r="K21" s="6" t="s">
@@ -9492,7 +9440,7 @@
         <v>288</v>
       </c>
       <c r="M21" s="6"/>
-      <c r="N21" s="9">
+      <c r="N21" s="7">
         <v>21</v>
       </c>
     </row>
@@ -9511,7 +9459,7 @@
         <v>258</v>
       </c>
       <c r="H22" s="6"/>
-      <c r="I22" s="9">
+      <c r="I22" s="7">
         <v>13</v>
       </c>
       <c r="K22" s="6" t="s">
@@ -9521,7 +9469,7 @@
         <v>272</v>
       </c>
       <c r="M22" s="6"/>
-      <c r="N22" s="9">
+      <c r="N22" s="7">
         <v>22</v>
       </c>
     </row>
@@ -9540,7 +9488,7 @@
         <v>257</v>
       </c>
       <c r="H23" s="6"/>
-      <c r="I23" s="9">
+      <c r="I23" s="7">
         <v>16</v>
       </c>
       <c r="K23" s="6" t="s">
@@ -9550,7 +9498,7 @@
         <v>289</v>
       </c>
       <c r="M23" s="6"/>
-      <c r="N23" s="9">
+      <c r="N23" s="7">
         <v>22</v>
       </c>
     </row>
@@ -9569,7 +9517,7 @@
         <v>260</v>
       </c>
       <c r="H24" s="6"/>
-      <c r="I24" s="9">
+      <c r="I24" s="7">
         <v>21</v>
       </c>
     </row>
@@ -9588,7 +9536,7 @@
         <v>262</v>
       </c>
       <c r="H25" s="6"/>
-      <c r="I25" s="9">
+      <c r="I25" s="7">
         <v>1</v>
       </c>
     </row>
@@ -9607,7 +9555,7 @@
         <v>264</v>
       </c>
       <c r="H26" s="6"/>
-      <c r="I26" s="9">
+      <c r="I26" s="7">
         <v>15</v>
       </c>
     </row>
@@ -9626,7 +9574,7 @@
         <v>264</v>
       </c>
       <c r="H27" s="6"/>
-      <c r="I27" s="9">
+      <c r="I27" s="7">
         <v>15</v>
       </c>
     </row>
@@ -9638,7 +9586,7 @@
         <v>266</v>
       </c>
       <c r="H28" s="6"/>
-      <c r="I28" s="9">
+      <c r="I28" s="7">
         <v>15</v>
       </c>
     </row>
@@ -9650,7 +9598,7 @@
         <v>247</v>
       </c>
       <c r="H29" s="6"/>
-      <c r="I29" s="9">
+      <c r="I29" s="7">
         <v>4</v>
       </c>
     </row>
@@ -9662,7 +9610,7 @@
         <v>254</v>
       </c>
       <c r="H30" s="6"/>
-      <c r="I30" s="9">
+      <c r="I30" s="7">
         <v>2</v>
       </c>
     </row>

</xml_diff>